<commit_message>
FIx: change method to deleting existing charts
Avoiding error when there are no existing charts
</commit_message>
<xml_diff>
--- a/excel_operation/practice4.xlsx
+++ b/excel_operation/practice4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\compl\Documents\PowerShell\powershell_practice\excel_operation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A047FF-0B38-4617-86EF-806FC0B4E500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25ADAB98-033F-43E0-8098-EB3236EADE9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5760" yWindow="2436" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -213,41 +213,41 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>9.5658086928855024E-2</c:v>
+                  <c:v>0.85430830386756851</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.44815183910346601</c:v>
+                  <c:v>0.81925136589768621</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>8.9851944539849016E-2</c:v>
+                  <c:v>0.54910392785347195</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.36140174864501351</c:v>
+                  <c:v>0.62733799111137956</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.72757231497431551</c:v>
+                  <c:v>0.1584161341077549</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.38462381571380477</c:v>
+                  <c:v>0.89373830779883334</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.31231080931525279</c:v>
+                  <c:v>0.94863481068778777</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.98655725809189787</c:v>
+                  <c:v>0.60675653563872112</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.75182273058287263</c:v>
+                  <c:v>0.86133672544868256</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.99241465234806669</c:v>
+                  <c:v>6.4679129665216162E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E6CC-4772-8088-E2DC63C0C045}"/>
+              <c16:uniqueId val="{00000000-9FAB-492A-B11C-00193D5F0E44}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -260,8 +260,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="1641349152"/>
-        <c:axId val="1641348320"/>
+        <c:axId val="977602383"/>
+        <c:axId val="977602799"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -329,34 +329,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.79704684184204166</c:v>
+                  <c:v>0.61513747149748743</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.3357105511540066E-4</c:v>
+                  <c:v>0.98928611133516031</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.47198029635213312</c:v>
+                  <c:v>0.68693629846554061</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.69503237602641632</c:v>
+                  <c:v>0.94848837893045723</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.23598196840196983</c:v>
+                  <c:v>0.99458452634587702</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.60314947857817258</c:v>
+                  <c:v>0.18410489095694149</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.51469389941435328</c:v>
+                  <c:v>0.10173074243894609</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.5058181629644114</c:v>
+                  <c:v>0.35111402605107345</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.73633042341812538</c:v>
+                  <c:v>0.1325228309816654</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.10935522160334732</c:v>
+                  <c:v>0.46045646489675363</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -364,7 +364,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E6CC-4772-8088-E2DC63C0C045}"/>
+              <c16:uniqueId val="{00000001-9FAB-492A-B11C-00193D5F0E44}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -378,11 +378,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1632190128"/>
-        <c:axId val="1633960912"/>
+        <c:axId val="981746383"/>
+        <c:axId val="981748463"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1641349152"/>
+        <c:axId val="977602383"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -392,7 +392,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1641348320"/>
+        <c:crossAx val="977602799"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -400,7 +400,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1641348320"/>
+        <c:axId val="977602799"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -411,12 +411,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1641349152"/>
+        <c:crossAx val="977602383"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1633960912"/>
+        <c:axId val="981748463"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -426,12 +426,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1632190128"/>
+        <c:crossAx val="981746383"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="1632190128"/>
+        <c:axId val="981746383"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -441,7 +441,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1633960912"/>
+        <c:crossAx val="981748463"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -574,41 +574,41 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.40176845273459272</c:v>
+                  <c:v>0.68850548638797804</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.86091629280068116</c:v>
+                  <c:v>0.10255549293659094</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.65638649761578904</c:v>
+                  <c:v>0.30005765525318828</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1722583514159205</c:v>
+                  <c:v>0.57953762973804845</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.91607290485015402</c:v>
+                  <c:v>0.23321254910659661</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.87462543390499925</c:v>
+                  <c:v>0.44030857356398834</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.16151527987936842</c:v>
+                  <c:v>0.60989447384011397</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.70353261738115835</c:v>
+                  <c:v>0.27787488025105256</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.76649894188242373</c:v>
+                  <c:v>0.45713376145146833</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.86624325935364499</c:v>
+                  <c:v>0.37795934353001581</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-7855-4D09-A194-C38867E057E1}"/>
+              <c16:uniqueId val="{00000003-4F9A-48D8-918F-B5B518AD0ABD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -621,8 +621,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="1632189296"/>
-        <c:axId val="1632193456"/>
+        <c:axId val="981747631"/>
+        <c:axId val="981748047"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -690,34 +690,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.559837775402937</c:v>
+                  <c:v>0.87781023849864814</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.19103282584904768</c:v>
+                  <c:v>0.83194622407200725</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.76992652035381037</c:v>
+                  <c:v>0.15829563411967917</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.31069373784127119</c:v>
+                  <c:v>0.66357950373790742</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.54258823046751747</c:v>
+                  <c:v>0.5020132924382531</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.37899088975838535</c:v>
+                  <c:v>0.40012310029779186</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.4101954394155189E-2</c:v>
+                  <c:v>0.8582549736708146</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.2985374800561451E-2</c:v>
+                  <c:v>0.48974065196555694</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.66104855249489591</c:v>
+                  <c:v>0.66679931215861221</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.39383055508910259</c:v>
+                  <c:v>0.11818156663510149</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -725,7 +725,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-7855-4D09-A194-C38867E057E1}"/>
+              <c16:uniqueId val="{00000004-4F9A-48D8-918F-B5B518AD0ABD}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -739,11 +739,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1573303600"/>
-        <c:axId val="1632185968"/>
+        <c:axId val="982422207"/>
+        <c:axId val="981745135"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1632189296"/>
+        <c:axId val="981747631"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -753,7 +753,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1632193456"/>
+        <c:crossAx val="981748047"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -761,7 +761,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1632193456"/>
+        <c:axId val="981748047"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -772,12 +772,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1632189296"/>
+        <c:crossAx val="981747631"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1632185968"/>
+        <c:axId val="981745135"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -787,12 +787,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1573303600"/>
+        <c:crossAx val="982422207"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="1573303600"/>
+        <c:axId val="982422207"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -802,7 +802,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1632185968"/>
+        <c:crossAx val="981745135"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -935,41 +935,41 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.10990252289930103</c:v>
+                  <c:v>0.62142887708204508</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.75996558504033829</c:v>
+                  <c:v>0.71058547681872919</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.286159478940608</c:v>
+                  <c:v>0.36875239228328649</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.63427749930630994</c:v>
+                  <c:v>0.24613876190120443</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.98047439904959455</c:v>
+                  <c:v>0.769855195408922</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.55601050263564156</c:v>
+                  <c:v>0.1103268591078933</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.10155287671654234</c:v>
+                  <c:v>0.65423264584900109</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.57129213836557302</c:v>
+                  <c:v>8.7076973871759389E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.0368189869902684E-2</c:v>
+                  <c:v>0.98568344521998474</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.8433596533796686E-2</c:v>
+                  <c:v>0.82519805016460013</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-466A-40D4-85BE-25D975D4BABA}"/>
+              <c16:uniqueId val="{00000003-0107-4908-AC18-CF029B50A3F0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -982,8 +982,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="1573300688"/>
-        <c:axId val="1573304848"/>
+        <c:axId val="979296463"/>
+        <c:axId val="979296879"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1051,34 +1051,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.32900480316706726</c:v>
+                  <c:v>0.16465803868150497</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.34254403330647076</c:v>
+                  <c:v>0.35824521774624052</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.85698875823745457</c:v>
+                  <c:v>0.27894583818631347</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.53921068995892774</c:v>
+                  <c:v>9.5835879234604571E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.59396005720854672</c:v>
+                  <c:v>0.78590223686963168</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.30900355540697988</c:v>
+                  <c:v>0.84516934968078616</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.60971164388279631</c:v>
+                  <c:v>0.39640704164200857</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.45226557368151854</c:v>
+                  <c:v>0.99851696614584318</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.44152978585169622</c:v>
+                  <c:v>0.49231397052103687</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.85811811960956286</c:v>
+                  <c:v>5.8882276901092712E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1086,7 +1086,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-466A-40D4-85BE-25D975D4BABA}"/>
+              <c16:uniqueId val="{00000004-0107-4908-AC18-CF029B50A3F0}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1100,11 +1100,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1632107424"/>
-        <c:axId val="1345916288"/>
+        <c:axId val="979295215"/>
+        <c:axId val="979297295"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1573300688"/>
+        <c:axId val="979296463"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1114,7 +1114,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1573304848"/>
+        <c:crossAx val="979296879"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1122,7 +1122,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1573304848"/>
+        <c:axId val="979296879"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1133,12 +1133,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1573300688"/>
+        <c:crossAx val="979296463"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1345916288"/>
+        <c:axId val="979297295"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1148,12 +1148,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1632107424"/>
+        <c:crossAx val="979295215"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="1632107424"/>
+        <c:axId val="979295215"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1163,7 +1163,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1345916288"/>
+        <c:crossAx val="979297295"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1296,41 +1296,41 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.49718283813766728</c:v>
+                  <c:v>1.7878717162821411E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3047276875277856E-2</c:v>
+                  <c:v>0.21611981700807181</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.88837711095523364</c:v>
+                  <c:v>0.85845541860349228</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.49165852507756691</c:v>
+                  <c:v>0.25781636195218705</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.80911048109617401</c:v>
+                  <c:v>0.89438102497250027</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.72264053278042029</c:v>
+                  <c:v>4.116315244838975E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.7516135307505016E-2</c:v>
+                  <c:v>0.73935054702671388</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.30885309934645055</c:v>
+                  <c:v>0.72074243958059514</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.62870625212675491</c:v>
+                  <c:v>0.38932591463702237</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.35865293816503474</c:v>
+                  <c:v>0.93254702424339264</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EFCD-425A-AE82-2531F6EEFD0B}"/>
+              <c16:uniqueId val="{00000000-17C1-4EBE-9441-1424B1CC438A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1343,8 +1343,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="0"/>
-        <c:axId val="1641347904"/>
-        <c:axId val="1641348736"/>
+        <c:axId val="979294383"/>
+        <c:axId val="979296047"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1412,34 +1412,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.23805625541426056</c:v>
+                  <c:v>0.35280831210815922</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.70848612154341806</c:v>
+                  <c:v>0.50208041461215669</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.29586113789842694</c:v>
+                  <c:v>0.81186990923212299</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.4883278663346977E-2</c:v>
+                  <c:v>0.76310121379182183</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.88336058019021502</c:v>
+                  <c:v>0.66735010635914382</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.11264981821913211</c:v>
+                  <c:v>0.69848028353848091</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.3839504669355174E-3</c:v>
+                  <c:v>0.60499129679612718</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.383769572854638E-2</c:v>
+                  <c:v>0.36928006760104459</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.2256249026017042</c:v>
+                  <c:v>0.97215719937634004</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.97393968174341738</c:v>
+                  <c:v>0.10928877173575757</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1447,7 +1447,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-EFCD-425A-AE82-2531F6EEFD0B}"/>
+              <c16:uniqueId val="{00000001-17C1-4EBE-9441-1424B1CC438A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1461,11 +1461,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1349328416"/>
-        <c:axId val="1349329664"/>
+        <c:axId val="979642127"/>
+        <c:axId val="979295631"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1641347904"/>
+        <c:axId val="979294383"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1475,7 +1475,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1641348736"/>
+        <c:crossAx val="979296047"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1483,7 +1483,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1641348736"/>
+        <c:axId val="979296047"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1494,12 +1494,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1641347904"/>
+        <c:crossAx val="979294383"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1349329664"/>
+        <c:axId val="979295631"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1509,12 +1509,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1349328416"/>
+        <c:crossAx val="979642127"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:catAx>
-        <c:axId val="1349328416"/>
+        <c:axId val="979642127"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1524,7 +1524,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1349329664"/>
+        <c:crossAx val="979295631"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -1571,10 +1571,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="グラフ 2">
+        <xdr:cNvPr id="2" name="グラフ 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6CF72C7-12D1-470A-933A-13AC7125ECE1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63DD9F67-40B6-41F4-B9F6-2F3740216D0B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1612,10 +1612,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="グラフ 1">
+        <xdr:cNvPr id="3" name="グラフ 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2BA7AA4-2D60-46E6-B724-DD353555F292}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70D80BBC-66D9-4977-9294-10044AF2AE68}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1653,10 +1653,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="グラフ 1">
+        <xdr:cNvPr id="3" name="グラフ 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26A0AA3C-4744-4267-AEC0-28A93FB08F44}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8FC3B2C-D48A-4268-A6E2-8FE88A315735}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1694,10 +1694,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="グラフ 1">
+        <xdr:cNvPr id="3" name="グラフ 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F73B46D-FEEA-4C85-A45E-5F0ACA901E8F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F30857A0-5CA9-472E-9180-DE9E657AB3BC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2006,11 +2006,11 @@
       </c>
       <c r="B17">
         <f ca="1">RAND()</f>
-        <v>9.5658086928855024E-2</v>
+        <v>0.85430830386756851</v>
       </c>
       <c r="C17">
         <f ca="1">RAND()</f>
-        <v>0.79704684184204166</v>
+        <v>0.61513747149748743</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2019,11 +2019,11 @@
       </c>
       <c r="B18">
         <f t="shared" ref="B18:C26" ca="1" si="0">RAND()</f>
-        <v>0.44815183910346601</v>
+        <v>0.81925136589768621</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>7.3357105511540066E-4</v>
+        <v>0.98928611133516031</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2032,11 +2032,11 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>8.9851944539849016E-2</v>
+        <v>0.54910392785347195</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.47198029635213312</v>
+        <v>0.68693629846554061</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2045,11 +2045,11 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.36140174864501351</v>
+        <v>0.62733799111137956</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.69503237602641632</v>
+        <v>0.94848837893045723</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2058,11 +2058,11 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72757231497431551</v>
+        <v>0.1584161341077549</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.23598196840196983</v>
+        <v>0.99458452634587702</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2071,11 +2071,11 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.38462381571380477</v>
+        <v>0.89373830779883334</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.60314947857817258</v>
+        <v>0.18410489095694149</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2084,11 +2084,11 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31231080931525279</v>
+        <v>0.94863481068778777</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.51469389941435328</v>
+        <v>0.10173074243894609</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2097,11 +2097,11 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.98655725809189787</v>
+        <v>0.60675653563872112</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.5058181629644114</v>
+        <v>0.35111402605107345</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2110,11 +2110,11 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.75182273058287263</v>
+        <v>0.86133672544868256</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.73633042341812538</v>
+        <v>0.1325228309816654</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2123,11 +2123,11 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.99241465234806669</v>
+        <v>6.4679129665216162E-2</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10935522160334732</v>
+        <v>0.46045646489675363</v>
       </c>
     </row>
   </sheetData>
@@ -2164,11 +2164,11 @@
       </c>
       <c r="B17">
         <f ca="1">RAND()</f>
-        <v>0.40176845273459272</v>
+        <v>0.68850548638797804</v>
       </c>
       <c r="C17">
         <f ca="1">RAND()</f>
-        <v>0.559837775402937</v>
+        <v>0.87781023849864814</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2177,11 +2177,11 @@
       </c>
       <c r="B18">
         <f t="shared" ref="B18:C26" ca="1" si="0">RAND()</f>
-        <v>0.86091629280068116</v>
+        <v>0.10255549293659094</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.19103282584904768</v>
+        <v>0.83194622407200725</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2190,11 +2190,11 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.65638649761578904</v>
+        <v>0.30005765525318828</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.76992652035381037</v>
+        <v>0.15829563411967917</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2203,11 +2203,11 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.1722583514159205</v>
+        <v>0.57953762973804845</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.31069373784127119</v>
+        <v>0.66357950373790742</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2216,11 +2216,11 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.91607290485015402</v>
+        <v>0.23321254910659661</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.54258823046751747</v>
+        <v>0.5020132924382531</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2229,11 +2229,11 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.87462543390499925</v>
+        <v>0.44030857356398834</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.37899088975838535</v>
+        <v>0.40012310029779186</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2242,11 +2242,11 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.16151527987936842</v>
+        <v>0.60989447384011397</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4101954394155189E-2</v>
+        <v>0.8582549736708146</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2255,11 +2255,11 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.70353261738115835</v>
+        <v>0.27787488025105256</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>8.2985374800561451E-2</v>
+        <v>0.48974065196555694</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2268,11 +2268,11 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.76649894188242373</v>
+        <v>0.45713376145146833</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.66104855249489591</v>
+        <v>0.66679931215861221</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2281,11 +2281,11 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.86624325935364499</v>
+        <v>0.37795934353001581</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.39383055508910259</v>
+        <v>0.11818156663510149</v>
       </c>
     </row>
   </sheetData>
@@ -2322,11 +2322,11 @@
       </c>
       <c r="B17">
         <f ca="1">RAND()</f>
-        <v>0.10990252289930103</v>
+        <v>0.62142887708204508</v>
       </c>
       <c r="C17">
         <f ca="1">RAND()</f>
-        <v>0.32900480316706726</v>
+        <v>0.16465803868150497</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2335,11 +2335,11 @@
       </c>
       <c r="B18">
         <f t="shared" ref="B18:C26" ca="1" si="0">RAND()</f>
-        <v>0.75996558504033829</v>
+        <v>0.71058547681872919</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.34254403330647076</v>
+        <v>0.35824521774624052</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2348,11 +2348,11 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.286159478940608</v>
+        <v>0.36875239228328649</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85698875823745457</v>
+        <v>0.27894583818631347</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2361,11 +2361,11 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.63427749930630994</v>
+        <v>0.24613876190120443</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.53921068995892774</v>
+        <v>9.5835879234604571E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2374,11 +2374,11 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.98047439904959455</v>
+        <v>0.769855195408922</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.59396005720854672</v>
+        <v>0.78590223686963168</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2387,11 +2387,11 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.55601050263564156</v>
+        <v>0.1103268591078933</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30900355540697988</v>
+        <v>0.84516934968078616</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2400,11 +2400,11 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.10155287671654234</v>
+        <v>0.65423264584900109</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>0.60971164388279631</v>
+        <v>0.39640704164200857</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2413,11 +2413,11 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.57129213836557302</v>
+        <v>8.7076973871759389E-2</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.45226557368151854</v>
+        <v>0.99851696614584318</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2426,11 +2426,11 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>8.0368189869902684E-2</v>
+        <v>0.98568344521998474</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.44152978585169622</v>
+        <v>0.49231397052103687</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2439,11 +2439,11 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>9.8433596533796686E-2</v>
+        <v>0.82519805016460013</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.85811811960956286</v>
+        <v>5.8882276901092712E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2480,11 +2480,11 @@
       </c>
       <c r="B17">
         <f ca="1">RAND()</f>
-        <v>0.49718283813766728</v>
+        <v>1.7878717162821411E-3</v>
       </c>
       <c r="C17">
         <f ca="1">RAND()</f>
-        <v>0.23805625541426056</v>
+        <v>0.35280831210815922</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2493,11 +2493,11 @@
       </c>
       <c r="B18">
         <f t="shared" ref="B18:C26" ca="1" si="0">RAND()</f>
-        <v>2.3047276875277856E-2</v>
+        <v>0.21611981700807181</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>0.70848612154341806</v>
+        <v>0.50208041461215669</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2506,11 +2506,11 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88837711095523364</v>
+        <v>0.85845541860349228</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>0.29586113789842694</v>
+        <v>0.81186990923212299</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2519,11 +2519,11 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>0.49165852507756691</v>
+        <v>0.25781636195218705</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>6.4883278663346977E-2</v>
+        <v>0.76310121379182183</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2532,11 +2532,11 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.80911048109617401</v>
+        <v>0.89438102497250027</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>0.88336058019021502</v>
+        <v>0.66735010635914382</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2545,11 +2545,11 @@
       </c>
       <c r="B22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.72264053278042029</v>
+        <v>4.116315244838975E-2</v>
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>0.11264981821913211</v>
+        <v>0.69848028353848091</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2558,11 +2558,11 @@
       </c>
       <c r="B23">
         <f t="shared" ca="1" si="0"/>
-        <v>8.7516135307505016E-2</v>
+        <v>0.73935054702671388</v>
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="0"/>
-        <v>6.3839504669355174E-3</v>
+        <v>0.60499129679612718</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2571,11 +2571,11 @@
       </c>
       <c r="B24">
         <f t="shared" ca="1" si="0"/>
-        <v>0.30885309934645055</v>
+        <v>0.72074243958059514</v>
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="0"/>
-        <v>8.383769572854638E-2</v>
+        <v>0.36928006760104459</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2584,11 +2584,11 @@
       </c>
       <c r="B25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.62870625212675491</v>
+        <v>0.38932591463702237</v>
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="0"/>
-        <v>0.2256249026017042</v>
+        <v>0.97215719937634004</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2597,11 +2597,11 @@
       </c>
       <c r="B26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.35865293816503474</v>
+        <v>0.93254702424339264</v>
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="0"/>
-        <v>0.97393968174341738</v>
+        <v>0.10928877173575757</v>
       </c>
     </row>
   </sheetData>

</xml_diff>